<commit_message>
Change colors and label
</commit_message>
<xml_diff>
--- a/madison_skills.xlsx
+++ b/madison_skills.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madis\Documents\madisonestabrook.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madis\Documents\GitHub\madisonestabrook.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0507CA-895A-46B7-B183-FDEB44470CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C6A843-29F1-429C-8CC3-16D8765274A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AA2A871-433D-4A58-B61D-1F3574CDF950}"/>
   </bookViews>
@@ -90,10 +90,10 @@
     <t>professional experience (years)</t>
   </si>
   <si>
-    <t>relative strength</t>
-  </si>
-  <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>mastery</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{EEC112E1-06B2-4F50-BA1E-720F908D1AEB}" name="Language"/>
     <tableColumn id="1" xr3:uid="{4FD69853-DD32-4AC7-BFEB-5DF0552E36D2}" name="skill"/>
-    <tableColumn id="2" xr3:uid="{DB49926F-4928-4943-8C14-A4CD674A6BCB}" name="relative strength"/>
+    <tableColumn id="2" xr3:uid="{DB49926F-4928-4943-8C14-A4CD674A6BCB}" name="mastery"/>
     <tableColumn id="3" xr3:uid="{3C232945-DD43-4FED-BA45-277C10E11803}" name="professional experience (years)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,13 +477,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Hopefully final touches. Add open-source contrib and DQ cert as well as new DBA skills
</commit_message>
<xml_diff>
--- a/madison_skills.xlsx
+++ b/madison_skills.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madis\Documents\GitHub\madisonestabrook.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C6A843-29F1-429C-8CC3-16D8765274A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF594C7E-57CA-4B98-AA9B-5B1C5606D23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AA2A871-433D-4A58-B61D-1F3574CDF950}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AA2A871-433D-4A58-B61D-1F3574CDF950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSciSkils" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>skill</t>
   </si>
@@ -94,6 +95,33 @@
   </si>
   <si>
     <t>mastery</t>
+  </si>
+  <si>
+    <t>Python task automation</t>
+  </si>
+  <si>
+    <t>PowerShell task automation</t>
+  </si>
+  <si>
+    <t>Optimize SQL performance</t>
+  </si>
+  <si>
+    <t>Information security</t>
+  </si>
+  <si>
+    <t>SQL Server Management Studio (SSMS)</t>
+  </si>
+  <si>
+    <t>Secure coding</t>
+  </si>
+  <si>
+    <t>Embedded SQL</t>
+  </si>
+  <si>
+    <t>Technical communication</t>
+  </si>
+  <si>
+    <t>Database design and data modeling</t>
   </si>
 </sst>
 </file>
@@ -149,17 +177,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B13DD4C3-63AD-4B6C-A627-CCE15E4FCA91}" name="Table1" displayName="Table1" ref="A1:D17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B13DD4C3-63AD-4B6C-A627-CCE15E4FCA91}" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{B13DD4C3-63AD-4B6C-A627-CCE15E4FCA91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
+    <sortCondition descending="1" ref="B2:B10"/>
+    <sortCondition descending="1" ref="C2:C10"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4FD69853-DD32-4AC7-BFEB-5DF0552E36D2}" name="skill"/>
+    <tableColumn id="2" xr3:uid="{DB49926F-4928-4943-8C14-A4CD674A6BCB}" name="mastery"/>
+    <tableColumn id="3" xr3:uid="{3C232945-DD43-4FED-BA45-277C10E11803}" name="professional experience (years)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD02F6FB-E9ED-45BE-BEE8-02D334D4769B}" name="Table13" displayName="Table13" ref="A1:D17" totalsRowShown="0">
   <autoFilter ref="A1:D17" xr:uid="{B13DD4C3-63AD-4B6C-A627-CCE15E4FCA91}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
     <sortCondition descending="1" ref="A12:A17"/>
     <sortCondition descending="1" ref="C12:C17"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{EEC112E1-06B2-4F50-BA1E-720F908D1AEB}" name="Language"/>
-    <tableColumn id="1" xr3:uid="{4FD69853-DD32-4AC7-BFEB-5DF0552E36D2}" name="skill"/>
-    <tableColumn id="2" xr3:uid="{DB49926F-4928-4943-8C14-A4CD674A6BCB}" name="mastery"/>
-    <tableColumn id="3" xr3:uid="{3C232945-DD43-4FED-BA45-277C10E11803}" name="professional experience (years)"/>
+    <tableColumn id="4" xr3:uid="{4997EE4D-2EAA-476F-87EA-A50382A7DCC7}" name="Language"/>
+    <tableColumn id="1" xr3:uid="{42FB0ECE-1693-403A-B019-F87405ECB618}" name="skill"/>
+    <tableColumn id="2" xr3:uid="{5088A893-5B7C-43AE-8C96-FBDB564E6637}" name="mastery"/>
+    <tableColumn id="3" xr3:uid="{C8A431DD-6F2B-49AE-9623-275E07A540E6}" name="professional experience (years)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,10 +506,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F887BF21-09D8-44B9-8080-7C4B0F1991C9}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>9.5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>8.5</v>
+      </c>
+      <c r="C6">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>3.5</v>
+      </c>
+      <c r="C10">
+        <v>0.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20EB9E3-343D-4BD2-AB90-0A76331B7EAA}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>